<commit_message>
Svalbard SimplyQ: version used for Svalbard Science Conference 2023
</commit_message>
<xml_diff>
--- a/models/data/Svalbard/HBV_Adventelva_runoff_2015_and_2016.xlsx
+++ b/models/data/Svalbard/HBV_Adventelva_runoff_2015_and_2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niva365-my.sharepoint.com/personal/leah_jackson-blake_niva_no/Documents/Data/Svalbard/Modelling/HBV_Aga/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\Mobius2\models\data\Svalbard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{3D4DCF13-0D2A-3641-95E0-BA006715872F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF64A509-1D8E-42DF-8B1E-4A2FD9918EC2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DE2A9B-0F52-4020-AA30-A2E299557799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="1356" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12156" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,16 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Electrical Conductivity (uS/cm)</t>
+    <t>HBV_Q_no winter runoff (m3/s)</t>
   </si>
   <si>
-    <t>Temperature (oC)</t>
+    <t>HBV_Q (m3/s)</t>
   </si>
   <si>
-    <t>Q with no winter runoff (m3/s)</t>
+    <t>UNIS_conductivity (uS/cm)</t>
   </si>
   <si>
-    <t>Q with winter runoff (m3/s)</t>
+    <t>UNIS_Temp</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:E732"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,16 +385,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>